<commit_message>
popup backlog subject matched
</commit_message>
<xml_diff>
--- a/TestDataFile/StudentBasicDetails.xlsx
+++ b/TestDataFile/StudentBasicDetails.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amity.DESKTOP-HKLU73H\git\selenium-studentportal\TestDataFile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amit.yadav.ext\git\selenium-studentportal\TestDataFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07D9B88-EC4D-4B3A-9005-A91F40ED214F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575"/>
+    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Details" sheetId="1" r:id="rId1"/>
@@ -29,20 +30,20 @@
     <t>Student Details</t>
   </si>
   <si>
-    <t>Shiv.Golani.Ext@nmims.edu</t>
+    <t>darshanchawade@gmail.com</t>
   </si>
   <si>
-    <t>MBA (FM)</t>
+    <t>MBA (ITSM)</t>
   </si>
   <si>
-    <t>Validity End: 31-Dec-2025</t>
+    <t>Validity End: 30-Jun-2026</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,6 +56,14 @@
       <color rgb="FF000000"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -95,25 +104,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -391,31 +402,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>8287324844</v>
+        <v>7709182030</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -425,7 +436,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>77777777775</v>
+        <v>77122558691</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
@@ -434,7 +445,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{1C2D4D9F-7668-4FC9-A69B-75BE568DBEE1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>